<commit_message>
Ejercico de Normalizacion y de Modelo Fiscio
</commit_message>
<xml_diff>
--- a/Normalizacion/Normalizacion.xlsx
+++ b/Normalizacion/Normalizacion.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelperez/Desktop/UNIVERSAE/GESTION DE BASE DE DATOS/Temario/Ejercicios/Normalizacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7734DFC3-2571-064B-8B5D-C7782341E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DF050E-8819-994D-ABEB-E77413E22359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{B089EB9E-B8E9-BC4A-BBDB-5CA565FEFD8D}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17760" activeTab="1" xr2:uid="{B089EB9E-B8E9-BC4A-BBDB-5CA565FEFD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalizacion1" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalizacion2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="61">
   <si>
     <t>ID_Piloto</t>
   </si>
@@ -144,13 +145,88 @@
   </si>
   <si>
     <t>3 FN</t>
+  </si>
+  <si>
+    <t>Nfactura</t>
+  </si>
+  <si>
+    <t>CodigoCliente</t>
+  </si>
+  <si>
+    <t>NombreCliente</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>CodigoProducto</t>
+  </si>
+  <si>
+    <t>NombreProducto</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>A2021/001</t>
+  </si>
+  <si>
+    <t>Frutales S.A</t>
+  </si>
+  <si>
+    <t>Caja Botellas Cristal</t>
+  </si>
+  <si>
+    <t>Caja Botellas Cristal, Vasos de plastico</t>
+  </si>
+  <si>
+    <t>A2021/002</t>
+  </si>
+  <si>
+    <t>A2021/003</t>
+  </si>
+  <si>
+    <t>kit de limpieza</t>
+  </si>
+  <si>
+    <t>Hermanos Antonio SL</t>
+  </si>
+  <si>
+    <t>Mantel gris, caja botellas cristal</t>
+  </si>
+  <si>
+    <t>C/Palomares 25 ,Madrid</t>
+  </si>
+  <si>
+    <t>C/Palomares 26, Madrid</t>
+  </si>
+  <si>
+    <t>C/Asza 24, Zaragoza</t>
+  </si>
+  <si>
+    <t>1FN</t>
+  </si>
+  <si>
+    <t>Vasos de plastico</t>
+  </si>
+  <si>
+    <t>Mantel gris</t>
+  </si>
+  <si>
+    <t>caja botellas cristal</t>
+  </si>
+  <si>
+    <t>2FN</t>
+  </si>
+  <si>
+    <t>YA ESTA EN 3 FN, NO HAY MAS DEPENDENCIAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +248,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -223,11 +319,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,18 +349,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,9 +715,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D7C83A-7071-F14B-BF2F-C7C07F19E2CB}">
-  <dimension ref="B2:L47"/>
+  <dimension ref="B2:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -756,7 +883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>2</v>
       </c>
@@ -773,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>3</v>
       </c>
@@ -790,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>3</v>
       </c>
@@ -807,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>4</v>
       </c>
@@ -824,19 +951,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="27" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="27" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
@@ -855,12 +975,11 @@
       <c r="H25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="9"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <v>1</v>
       </c>
@@ -879,12 +998,11 @@
       <c r="H26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <v>2</v>
       </c>
@@ -903,12 +1021,11 @@
       <c r="H27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <v>3</v>
       </c>
@@ -927,12 +1044,11 @@
       <c r="H28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <v>4</v>
       </c>
@@ -951,12 +1067,8 @@
       <c r="H29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E30" s="3">
         <v>3</v>
       </c>
@@ -970,7 +1082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E31" s="3">
         <v>4</v>
       </c>
@@ -984,42 +1096,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-    </row>
-    <row r="35" spans="2:12" ht="27" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="35" spans="2:11" ht="27" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="7"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
@@ -1039,8 +1127,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B38" s="8">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="6">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1055,12 +1143,12 @@
       <c r="G38" s="3">
         <v>1</v>
       </c>
-      <c r="H38" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="8">
+      <c r="H38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="6">
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1075,11 +1163,11 @@
       <c r="G39" s="3">
         <v>1</v>
       </c>
-      <c r="H39" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H39" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="3">
         <v>3</v>
       </c>
@@ -1099,45 +1187,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="G41" s="3">
         <v>3</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
       <c r="G42" s="3">
         <v>3</v>
       </c>
-      <c r="H42" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="G43" s="3">
         <v>4</v>
       </c>
-      <c r="H43" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="3">
         <v>1</v>
       </c>
@@ -1145,7 +1232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="3">
         <v>2</v>
       </c>
@@ -1153,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="3">
         <v>3</v>
       </c>
@@ -1161,7 +1248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="3">
         <v>4</v>
       </c>
@@ -1172,4 +1259,442 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C7D230-AA36-8343-BADE-1251C9D8E691}">
+  <dimension ref="B4:H48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1010.1026000000001</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="9">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2288</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="9">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="8">
+        <v>908.101</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="9">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="27" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1010</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="9">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1026</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="9">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2288</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="9">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="8">
+        <v>908</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="9">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1010</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="12">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1010</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="11">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1026</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="F30" s="8">
+        <v>2288</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="F31" s="8">
+        <v>908</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G32" s="16"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1010</v>
+      </c>
+      <c r="F37" s="9">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1026</v>
+      </c>
+      <c r="F38" s="9">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="8">
+        <v>2</v>
+      </c>
+      <c r="E39" s="8">
+        <v>2288</v>
+      </c>
+      <c r="F39" s="9">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="8">
+        <v>2</v>
+      </c>
+      <c r="E40" s="8">
+        <v>908</v>
+      </c>
+      <c r="F40" s="9">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="11">
+        <v>2</v>
+      </c>
+      <c r="E41" s="11">
+        <v>1010</v>
+      </c>
+      <c r="F41" s="12">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="B47" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C48:E48"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>